<commit_message>
v6 optimized( - global + HTTPAdapter)
</commit_message>
<xml_diff>
--- a/Parser_YD_GOO.xlsx
+++ b/Parser_YD_GOO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13365" windowHeight="3525"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5625"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,311 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="100">
+  <si>
+    <t>п\п</t>
+  </si>
+  <si>
+    <t>Ключ</t>
+  </si>
+  <si>
+    <t>Название компании</t>
+  </si>
+  <si>
+    <t>Позиция</t>
+  </si>
+  <si>
+    <t>Ссылка</t>
+  </si>
+  <si>
+    <t>Быстрая</t>
+  </si>
+  <si>
+    <t>Описалово</t>
+  </si>
+  <si>
+    <t>Контакты</t>
+  </si>
+  <si>
+    <t>﻿бухгалтерские услуги</t>
+  </si>
+  <si>
+    <t>Бухгалтерское обслуживание – От 1 175р./мес.</t>
+  </si>
+  <si>
+    <t>bo.1cborc.ru</t>
+  </si>
+  <si>
+    <t>Экспресс-аудит бухучетаТарифыМат. ответ-ть350+ довольных клиентов</t>
+  </si>
+  <si>
+    <t>Лицензия 1С включена в стоимость. Грамотное ведение бух. и нал. учета ООО и ИП. · Расчет заработной платы. Учет кадров. Расчет налогов. Составление отчетности. Сдача нулевой отчетности. Рег-я/ликвидация ООО/ИП</t>
+  </si>
+  <si>
+    <t>+7 (812) 385-15-85</t>
+  </si>
+  <si>
+    <t>Бухгалтерские услуги. Комплекс – от 1200 ₽/мес в СПБ!</t>
+  </si>
+  <si>
+    <t>buhgalter.1cbo.ru</t>
+  </si>
+  <si>
+    <t>Комплекс от 1200₽/месОтчётность от 784₽/месПрограммы уже в тарифе</t>
+  </si>
+  <si>
+    <t>Доверьте бухучёт 1С:БО. 100% автоматизация сервиса, низкая стоимость. Качество! · 24500 клиентов. 724 партнёра. 204 города. 28 лет опыта. 830 отзывов</t>
+  </si>
+  <si>
+    <t>+7 (499) 976-15-11</t>
+  </si>
+  <si>
+    <t>Бухгалтерский учет – На аутсорсинге</t>
+  </si>
+  <si>
+    <t>bs47.ru</t>
+  </si>
+  <si>
+    <t>Связаться с намиО насУслуги1С в облаке</t>
+  </si>
+  <si>
+    <t>Бухгалтерский учет, оптимизация налогообложения. Профессиональный подход. Звоните! · Всегда на связи. Фин. гарантии. Постоплата по договору. Облачная 1С</t>
+  </si>
+  <si>
+    <t>+7 (911) 240-00-10</t>
+  </si>
+  <si>
+    <t>Бухгалтерские услуги – Консультация бесплатно!</t>
+  </si>
+  <si>
+    <t>nvk-consult.ru</t>
+  </si>
+  <si>
+    <t>Бухгалтерский учетЮридические услугиАудит компанийЦены на услуги</t>
+  </si>
+  <si>
+    <t>Ответим на вопросы по бухгалтерскому и налоговому учету. Составлению отчетности. · Весь спектр услуг. 13 лет опыта. Доступные цены. Уменьшаем налоги</t>
+  </si>
+  <si>
+    <t>+7 (812) 332-05-80</t>
+  </si>
+  <si>
+    <t>Бухгалтерские услуги – Мегаконсалт</t>
+  </si>
+  <si>
+    <t>megaconsult.ru</t>
+  </si>
+  <si>
+    <t>УслугиЦеныДля ИП от 3 400 руб/месДля ООО от 4 000 руб/мес</t>
+  </si>
+  <si>
+    <t>Говорим с клиентом на одном языке. С нами вы поймёте, за что отдаёте деньги. Звоните! · Налоговые консультации. Ведение кадров. Расчёт з/п. Эффективная бухгалтерия</t>
+  </si>
+  <si>
+    <t>+7 (812) 425-32-38</t>
+  </si>
+  <si>
+    <t>Бухгалтерские услуги в СПб – Под ключ.</t>
+  </si>
+  <si>
+    <t>efafinance-uslugi.ru</t>
+  </si>
+  <si>
+    <t>Бесплатная консультацияСтоимостьУслугиОтзывы</t>
+  </si>
+  <si>
+    <t>Цены от 1500 руб/месяц. 10 лет на рынке. Оставьте заявку на консультацию. · Быстро. Надежно. Комплексно</t>
+  </si>
+  <si>
+    <t>8 (800) 707-03-64</t>
+  </si>
+  <si>
+    <t>Бухгалтерские услуги – Со скидкой 50%</t>
+  </si>
+  <si>
+    <t>algras.ru</t>
+  </si>
+  <si>
+    <t>[Сравните цены][Ведение ООО и ИП][Получи 10%, 20%, 50%][C нуля]</t>
+  </si>
+  <si>
+    <t>1 месяц за пол цены! Работаем в онлайн режиме! Бухгалтерские услуги от 500 руб. · Весь цикл услуг. Отзывы. Отвечаем в теч 15-30 мин. Доступ к 1С 24/7</t>
+  </si>
+  <si>
+    <t>+7 (812) 317-22-07</t>
+  </si>
+  <si>
+    <t>Бухгалтерские услуги! / accountingfinance.ru</t>
+  </si>
+  <si>
+    <t>accountingfinance.ru</t>
+  </si>
+  <si>
+    <t>Профессиональная бухгалтерия под ключ от 1 000 рублей в месяц! Звоните!</t>
+  </si>
+  <si>
+    <t>+7 (812) 309-98-35</t>
+  </si>
+  <si>
+    <t>Бухгалтерские услуги в СПб – Акция: подарок на выбор</t>
+  </si>
+  <si>
+    <t>декларация.com</t>
+  </si>
+  <si>
+    <t>Аутсорсинг бухгалтерииКонсалтингРекрутинг и КДПАудит бухгалтерии</t>
+  </si>
+  <si>
+    <t>Бухгалтерские услуги. Решаем сложные вопросы в сжатые сроки. Детально консультируем! · Гибкие цены. Правильная консультация. Точно в срок. Качественно</t>
+  </si>
+  <si>
+    <t>+7 (981) 802-26-69</t>
+  </si>
+  <si>
+    <t>Бухгалтерские услуги. – Сдача отчётности ИП и ООО</t>
+  </si>
+  <si>
+    <t>moedelo.org</t>
+  </si>
+  <si>
+    <t>Снижаем налогиБесплатный демо-доступООО и ИПСтрахуем на 100 млн.</t>
+  </si>
+  <si>
+    <t>Бухгалтерские услуги. Законно снижаем налоги. Компания «Моё дело». Кликай. · Поддержка 24/7. Цена. Отчетность ООО. Отчетность ИП</t>
+  </si>
+  <si>
+    <t>+7 (800) 200-77-27</t>
+  </si>
+  <si>
+    <t>бухгалтерский аудит</t>
+  </si>
+  <si>
+    <t>Бухгалтерский аудит от 1С:БО – за 4 часа бесплатно!</t>
+  </si>
+  <si>
+    <t>Как избежать штрафовАудит нужен или нетУдобный форматОт вас заявка</t>
+  </si>
+  <si>
+    <t>Пройдите бесплатно экспресс-аудит 1С:БухОбслуживание и наведите порядок в бухучете! · Аудит бесплатно. Быстро за 4 часа. Помощь в бухучете. Конфиденциально · 18+</t>
+  </si>
+  <si>
+    <t>Бухгалтерский аудит – с «Бизнес Консалт»</t>
+  </si>
+  <si>
+    <t>bkonsalt.ru</t>
+  </si>
+  <si>
+    <t>Обязательный аудитИнициативный аудитАудит по МСФОГарантировано</t>
+  </si>
+  <si>
+    <t>Независимое аудит-заключение с сохранением тайны! Работаем с 2011 г. Узнайте цены! · Стаж более 10 лет. Член СРО аудиторов. Консультации бесплатно</t>
+  </si>
+  <si>
+    <t>+7 (812) 449-42-90</t>
+  </si>
+  <si>
+    <t>Аудиторское заключение 30 тыс.руб.! / irene-audit.ru</t>
+  </si>
+  <si>
+    <t>irene-audit.ru</t>
+  </si>
+  <si>
+    <t>Успейте заключить договор на аудит для сдачи баланса до 6 апреля!</t>
+  </si>
+  <si>
+    <t>Обязательный бухгалтерский аудит – Закажите онлайн!</t>
+  </si>
+  <si>
+    <t>pia.ru</t>
+  </si>
+  <si>
+    <t>Юридические услугиУслуги по оценкеКонсалтингУслуги аудита</t>
+  </si>
+  <si>
+    <t>Лицензия ФСБ РФ. Прошли плановые проверки СРО. Контроль качества! Санкт-Петербург. · Доступные цены. Работаем 25 лет. Профессионально. Опытный персонал</t>
+  </si>
+  <si>
+    <t>+7 (812) 297-45-01</t>
+  </si>
+  <si>
+    <t>Сдача бухгалтерской отчетности – 1600₽/г - все включено!</t>
+  </si>
+  <si>
+    <t>taxcom.ru</t>
+  </si>
+  <si>
+    <t>Эл. документооборотЭЦП за 0 ₽Такском-ИнформерКалендарь бухгалтера</t>
+  </si>
+  <si>
+    <t>Быстрая и удобная сдача отчетов. Проверка на ошибки. Уведомления на телефон. · 20 лет опыта. Доверие 800000 клиентов. Отчет без ошибок</t>
+  </si>
+  <si>
+    <t>+7 (800) 300-64-86</t>
+  </si>
+  <si>
+    <t>Аудит 30 тыс.руб.! Онлайн / audit-search.ru</t>
+  </si>
+  <si>
+    <t>audit-search.ru</t>
+  </si>
+  <si>
+    <t>Не покупайте аудит пока не узнаете цену у нас! Гарантии возврата денег! Вся Россия!</t>
+  </si>
+  <si>
+    <t>Аутсорсинг бухгалтерских услуг в Москве, цены...</t>
+  </si>
+  <si>
+    <t>Снижение налоговКонтроль учетаИП и ОООСтрахуем на 100 млн</t>
+  </si>
+  <si>
+    <t>Команда аутсорсинг-бухгалтеров под вашу отрасль. Удобное приложение для контроля. · Бухгалтер. Юрист. Бизнес-ассистент. Оптимизация налогов. Удалённая бухгалтерия</t>
+  </si>
+  <si>
+    <t>Аудит бухгалтерии – от 450 руб/мес для ИП и ООО</t>
+  </si>
+  <si>
+    <t>авизопрофи.рф</t>
+  </si>
+  <si>
+    <t>Скидки и акцииДля нового бизнесаНаш опыт работыКак мы работаем</t>
+  </si>
+  <si>
+    <t>Качественный аутсорсинг бухгалтерии. Оптимизация расходов. Поддержка 24/7. Звоните! · Исключаем штрафы. Ежемесячные отчеты. Бесплатные консультации. Матер. ответственность</t>
+  </si>
+  <si>
+    <t>+7 (982) 696-35-40</t>
+  </si>
+  <si>
+    <t>Аудиторские услуги. 24 года опыта! / finauditservice.ru</t>
+  </si>
+  <si>
+    <t>finauditservice.ru</t>
+  </si>
+  <si>
+    <t>О насУслугиОтзывыКонтакты</t>
+  </si>
+  <si>
+    <t>АКГ "Финаудитсервис". Высокое качество! Разумные цены! Обращайтесь!</t>
+  </si>
+  <si>
+    <t>+7 (499) 397-85-35</t>
+  </si>
+  <si>
+    <t>Работа бухгалтером по зарплате в Санкт-Петербурге...</t>
+  </si>
+  <si>
+    <t>spb.rabota.ru</t>
+  </si>
+  <si>
+    <t>Свежие вакансииСоздать резюмеПоиск по компаниямПоиск по профессиям</t>
+  </si>
+  <si>
+    <t>Только проверенные и актуальные вакансии от прямых работодателей. Оставьте отклик! · Работа без опыта. Работа для студентов. Подработка. Оформление по ТК</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -336,12 +641,541 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" t="s">
+        <v>77</v>
+      </c>
+      <c r="G16" t="s">
+        <v>78</v>
+      </c>
+      <c r="H16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20">
+        <v>18</v>
+      </c>
+      <c r="E20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" t="s">
+        <v>93</v>
+      </c>
+      <c r="G20" t="s">
+        <v>94</v>
+      </c>
+      <c r="H20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21">
+        <v>19</v>
+      </c>
+      <c r="E21" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>